<commit_message>
Modify traverseFolder to compare time of json file with other files so json file only update when it is not the latest
</commit_message>
<xml_diff>
--- a/forTesting/Testing 2.xlsx
+++ b/forTesting/Testing 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Dropbox (Personal)\Work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jason\Github\DuplicateFileManagementSystem\forTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t xml:space="preserve">Tool List </t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Model Name from Litech Catalogue</t>
+  </si>
+  <si>
+    <t>Testing</t>
   </si>
 </sst>
 </file>
@@ -430,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F11"/>
+  <dimension ref="B2:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,6 +543,11 @@
       </c>
       <c r="C11" s="4"/>
     </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
create function to compare 2 files byte by byte
</commit_message>
<xml_diff>
--- a/forTesting/Testing 2.xlsx
+++ b/forTesting/Testing 2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t xml:space="preserve">Tool List </t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>Model Name from Litech Catalogue</t>
-  </si>
-  <si>
-    <t>Testing</t>
   </si>
 </sst>
 </file>
@@ -433,7 +430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F12"/>
+  <dimension ref="B2:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
@@ -543,11 +540,6 @@
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>